<commit_message>
fix the cucumber test - failed to use customize class
</commit_message>
<xml_diff>
--- a/test/test-etl/test-data/holding-data.xlsx
+++ b/test/test-etl/test-data/holding-data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joeylam/repo/njs/njstool/test/test-etl/test-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1783377C-911F-914D-BB35-B11A9E3989FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF52A987-9939-1046-B055-30EB26276CDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="1000" windowWidth="27640" windowHeight="15260" xr2:uid="{691E18BC-4642-F048-BDA6-32E38C16FBDA}"/>
   </bookViews>
@@ -19,14 +19,6 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -420,7 +412,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>